<commit_message>
Update Burndown and GanttChart
Update Actual Time and Estimated Time, adding 'All Burndown' on Burndown chart, adding every sprint to Burndown
</commit_message>
<xml_diff>
--- a/Files/Burndown Chart.xlsx
+++ b/Files/Burndown Chart.xlsx
@@ -5,14 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\e-Tracer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muham\Desktop\Before Upload Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ALL-Burndown" sheetId="5" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sprint 2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint 3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sprint 4" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Task</t>
   </si>
@@ -111,6 +115,54 @@
   </si>
   <si>
     <t>17 maret</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>Halaman Alumni</t>
+  </si>
+  <si>
+    <t>Halaman Admin</t>
+  </si>
+  <si>
+    <t>Halaman Kuesioner Alumni</t>
+  </si>
+  <si>
+    <t>Halaman Kuesioner Perusahaan</t>
+  </si>
+  <si>
+    <t>Halaman Buat Berita</t>
+  </si>
+  <si>
+    <t>Halaman Berita</t>
+  </si>
+  <si>
+    <t>Halaman Login</t>
+  </si>
+  <si>
+    <t>Time (Hour)</t>
+  </si>
+  <si>
+    <t>Estimated Time</t>
+  </si>
+  <si>
+    <t>Actual Time</t>
+  </si>
+  <si>
+    <t>No Task</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
   </si>
 </sst>
 </file>
@@ -205,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -238,6 +290,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -256,6 +321,636 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown Sprint</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ALL-Burndown'!$E$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimated Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ALL-Burndown'!$D$8:$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ALL-Burndown'!$E$8:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2F89-400C-AAA9-657D5AC63217}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ALL-Burndown'!$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ALL-Burndown'!$D$8:$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ALL-Burndown'!$F$8:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2F89-400C-AAA9-657D5AC63217}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="390147360"/>
+        <c:axId val="390146376"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="390147360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="390146376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="390146376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="390147360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -334,7 +1029,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$12</c:f>
+              <c:f>'Sprint 1'!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -420,7 +1115,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$6:$R$6</c:f>
+              <c:f>'Sprint 1'!$D$6:$R$6</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -473,7 +1168,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$12:$R$12</c:f>
+              <c:f>'Sprint 1'!$C$12:$R$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -537,7 +1232,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$13</c:f>
+              <c:f>'Sprint 1'!$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -623,7 +1318,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$6:$R$6</c:f>
+              <c:f>'Sprint 1'!$D$6:$R$6</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -676,7 +1371,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$13:$R$13</c:f>
+              <c:f>'Sprint 1'!$C$13:$R$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -962,6 +1657,1200 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 2</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimated Time Remaining (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 2'!$D$5:$S$5</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Task</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time (Hour)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15-Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16-Mar</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17-Mar</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18-Mar</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19-Mar</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25-Mar</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26-Mar</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27-Mar</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28-Mar</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29-Mar</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>01-Apr</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>02-Apr</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>03-Apr</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>04-Apr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$D$14:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.285714285714292</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.571428571428584</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.857142857142868</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.142857142857153</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51.428571428571438</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.714285714285722</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34.285714285714292</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.571428571428577</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.857142857142861</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.142857142857146</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.7142857142857162</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-84C6-4B68-8CEF-FDFBCC7B721D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$C$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Time Remaining (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 2'!$D$5:$S$5</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Task</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time (Hour)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15-Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16-Mar</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17-Mar</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18-Mar</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19-Mar</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25-Mar</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26-Mar</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27-Mar</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28-Mar</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29-Mar</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>01-Apr</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>02-Apr</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>03-Apr</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>04-Apr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$D$15:$S$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-84C6-4B68-8CEF-FDFBCC7B721D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="390819008"/>
+        <c:axId val="390821304"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="390819008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="390821304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="390821304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="390819008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimated Time Remaining (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 2'!$D$5:$S$5</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Task</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time (Hour)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15-Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16-Mar</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17-Mar</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18-Mar</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19-Mar</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25-Mar</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26-Mar</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27-Mar</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28-Mar</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29-Mar</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>01-Apr</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>02-Apr</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>03-Apr</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>04-Apr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$D$14:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.285714285714292</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.571428571428584</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.857142857142868</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.142857142857153</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51.428571428571438</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.714285714285722</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34.285714285714292</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.571428571428577</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.857142857142861</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.142857142857146</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.7142857142857162</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0753-4EE2-9C86-C38CF39AC7C1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$C$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Time Remaining (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 2'!$D$5:$S$5</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Task</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time (Hour)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15-Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16-Mar</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17-Mar</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18-Mar</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19-Mar</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25-Mar</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26-Mar</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27-Mar</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28-Mar</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29-Mar</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>01-Apr</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>02-Apr</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>03-Apr</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>04-Apr</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$D$15:$S$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0753-4EE2-9C86-C38CF39AC7C1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="390819008"/>
+        <c:axId val="390821304"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="390819008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="390821304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="390821304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="390819008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1002,7 +2891,603 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="294">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1551,7 +4036,1112 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1578,6 +5168,73 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1849,10 +5506,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D7:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="10">
+        <v>68</v>
+      </c>
+      <c r="F8" s="10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="10">
+        <v>80</v>
+      </c>
+      <c r="F9" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,134 +5907,134 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="7">
         <f>SUM(D7:D11)</f>
         <v>68</v>
       </c>
       <c r="E12" s="7">
-        <f>D12-($D$12/14)</f>
+        <f t="shared" ref="E12:P12" si="0">D12-($D$12/14)</f>
         <v>63.142857142857146</v>
       </c>
       <c r="F12" s="7">
-        <f>E12-($D$12/14)</f>
+        <f t="shared" si="0"/>
         <v>58.285714285714292</v>
       </c>
       <c r="G12" s="7">
-        <f>F12-($D$12/14)</f>
+        <f t="shared" si="0"/>
         <v>53.428571428571438</v>
       </c>
       <c r="H12" s="7">
-        <f>G12-($D$12/14)</f>
+        <f t="shared" si="0"/>
         <v>48.571428571428584</v>
       </c>
       <c r="I12" s="7">
-        <f>H12-($D$12/14)</f>
+        <f t="shared" si="0"/>
         <v>43.71428571428573</v>
       </c>
       <c r="J12" s="7">
-        <f>I12-($D$12/14)</f>
+        <f t="shared" si="0"/>
         <v>38.857142857142875</v>
       </c>
       <c r="K12" s="7">
-        <f>J12-($D$12/14)</f>
+        <f t="shared" si="0"/>
         <v>34.000000000000021</v>
       </c>
       <c r="L12" s="7">
-        <f>K12-($D$12/14)</f>
+        <f t="shared" si="0"/>
         <v>29.142857142857164</v>
       </c>
       <c r="M12" s="7">
-        <f>L12-($D$12/14)</f>
+        <f t="shared" si="0"/>
         <v>24.285714285714306</v>
       </c>
       <c r="N12" s="7">
-        <f>M12-($D$12/14)</f>
+        <f t="shared" si="0"/>
         <v>19.428571428571448</v>
       </c>
       <c r="O12" s="7">
-        <f>N12-($D$12/14)</f>
+        <f t="shared" si="0"/>
         <v>14.571428571428591</v>
       </c>
       <c r="P12" s="7">
-        <f>O12-($D$12/14)</f>
+        <f t="shared" si="0"/>
         <v>9.7142857142857331</v>
       </c>
       <c r="Q12" s="7">
-        <f t="shared" ref="Q12:R12" si="0">P12-($D$12/14)</f>
+        <f t="shared" ref="Q12:R12" si="1">P12-($D$12/14)</f>
         <v>4.8571428571428763</v>
       </c>
       <c r="R12" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9539925233402755E-14</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="7">
         <f>SUM(D7:D11)</f>
         <v>68</v>
       </c>
       <c r="E13" s="7">
-        <f>D13-SUM(E7:E11)</f>
+        <f t="shared" ref="E13:P13" si="2">D13-SUM(E7:E11)</f>
         <v>66</v>
       </c>
       <c r="F13" s="7">
-        <f>E13-SUM(F7:F11)</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="G13" s="7">
-        <f>F13-SUM(G7:G11)</f>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="H13" s="7">
-        <f>G13-SUM(H7:H11)</f>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="I13" s="7">
-        <f>H13-SUM(I7:I11)</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="J13" s="7">
-        <f>I13-SUM(J7:J11)</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="K13" s="7">
-        <f>J13-SUM(K7:K11)</f>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="L13" s="7">
-        <f>K13-SUM(L7:L11)</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="M13" s="7">
-        <f>L13-SUM(M7:M11)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="N13" s="7">
-        <f>M13-SUM(N7:N11)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="O13" s="7">
-        <f>N13-SUM(O7:O11)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="P13" s="7">
-        <f>O13-SUM(P7:P11)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Q13" s="7">
-        <f t="shared" ref="Q13:R13" si="1">P13-SUM(Q7:Q11)</f>
+        <f t="shared" ref="Q13:R13" si="3">P13-SUM(Q7:Q11)</f>
         <v>0</v>
       </c>
       <c r="R13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2326,4 +6050,662 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:S15"/>
+  <sheetViews>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="15">
+        <v>43539</v>
+      </c>
+      <c r="G5" s="15">
+        <v>43540</v>
+      </c>
+      <c r="H5" s="15">
+        <v>43541</v>
+      </c>
+      <c r="I5" s="15">
+        <v>43542</v>
+      </c>
+      <c r="J5" s="15">
+        <v>43543</v>
+      </c>
+      <c r="K5" s="15">
+        <v>43549</v>
+      </c>
+      <c r="L5" s="15">
+        <v>43550</v>
+      </c>
+      <c r="M5" s="15">
+        <v>43551</v>
+      </c>
+      <c r="N5" s="15">
+        <v>43552</v>
+      </c>
+      <c r="O5" s="15">
+        <v>43553</v>
+      </c>
+      <c r="P5" s="15">
+        <v>43556</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>43557</v>
+      </c>
+      <c r="R5" s="15">
+        <v>43558</v>
+      </c>
+      <c r="S5" s="15">
+        <v>43559</v>
+      </c>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="4">
+        <v>8</v>
+      </c>
+      <c r="F6" s="9">
+        <v>2</v>
+      </c>
+      <c r="G6" s="9">
+        <v>2</v>
+      </c>
+      <c r="H6" s="9">
+        <v>2</v>
+      </c>
+      <c r="I6" s="9">
+        <v>2</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0</v>
+      </c>
+      <c r="M6" s="10">
+        <v>0</v>
+      </c>
+      <c r="N6" s="10">
+        <v>0</v>
+      </c>
+      <c r="O6" s="10">
+        <v>0</v>
+      </c>
+      <c r="P6" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>0</v>
+      </c>
+      <c r="R6" s="10">
+        <v>0</v>
+      </c>
+      <c r="S6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C7" s="14">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="4">
+        <v>4</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9">
+        <v>2</v>
+      </c>
+      <c r="J7" s="9">
+        <v>2</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0</v>
+      </c>
+      <c r="M7" s="10">
+        <v>0</v>
+      </c>
+      <c r="N7" s="10">
+        <v>0</v>
+      </c>
+      <c r="O7" s="10">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>0</v>
+      </c>
+      <c r="R7" s="10">
+        <v>0</v>
+      </c>
+      <c r="S7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C8" s="14">
+        <v>3</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="4">
+        <v>16</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>2</v>
+      </c>
+      <c r="J8" s="9">
+        <v>2</v>
+      </c>
+      <c r="K8" s="9">
+        <v>2</v>
+      </c>
+      <c r="L8" s="9">
+        <v>2</v>
+      </c>
+      <c r="M8" s="10">
+        <v>2</v>
+      </c>
+      <c r="N8" s="10">
+        <v>2</v>
+      </c>
+      <c r="O8" s="10">
+        <v>2</v>
+      </c>
+      <c r="P8" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>1</v>
+      </c>
+      <c r="R8" s="10">
+        <v>1</v>
+      </c>
+      <c r="S8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C9" s="14">
+        <v>4</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="4">
+        <v>16</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <v>2</v>
+      </c>
+      <c r="K9" s="9">
+        <v>2</v>
+      </c>
+      <c r="L9" s="9">
+        <v>2</v>
+      </c>
+      <c r="M9" s="10">
+        <v>2</v>
+      </c>
+      <c r="N9" s="10">
+        <v>2</v>
+      </c>
+      <c r="O9" s="10">
+        <v>2</v>
+      </c>
+      <c r="P9" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>2</v>
+      </c>
+      <c r="R9" s="10">
+        <v>2</v>
+      </c>
+      <c r="S9" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C10" s="14">
+        <v>5</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="5">
+        <v>16</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0</v>
+      </c>
+      <c r="I10" s="9">
+        <v>4</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0</v>
+      </c>
+      <c r="K10" s="9">
+        <v>0</v>
+      </c>
+      <c r="L10" s="9">
+        <v>0</v>
+      </c>
+      <c r="M10" s="10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="10">
+        <v>2</v>
+      </c>
+      <c r="O10" s="10">
+        <v>2</v>
+      </c>
+      <c r="P10" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>2</v>
+      </c>
+      <c r="R10" s="10">
+        <v>2</v>
+      </c>
+      <c r="S10" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C11" s="14">
+        <v>6</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="13">
+        <v>12</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>4</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0</v>
+      </c>
+      <c r="M11" s="10">
+        <v>0</v>
+      </c>
+      <c r="N11" s="10">
+        <v>2</v>
+      </c>
+      <c r="O11" s="10">
+        <v>2</v>
+      </c>
+      <c r="P11" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>2</v>
+      </c>
+      <c r="R11" s="10">
+        <v>2</v>
+      </c>
+      <c r="S11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C12" s="14">
+        <v>7</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="6">
+        <v>4</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0</v>
+      </c>
+      <c r="K12" s="9">
+        <v>0</v>
+      </c>
+      <c r="L12" s="9">
+        <v>0</v>
+      </c>
+      <c r="M12" s="9">
+        <v>0</v>
+      </c>
+      <c r="N12" s="9">
+        <v>0</v>
+      </c>
+      <c r="O12" s="10">
+        <v>1</v>
+      </c>
+      <c r="P12" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>1</v>
+      </c>
+      <c r="R12" s="10">
+        <v>1</v>
+      </c>
+      <c r="S12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C13" s="14">
+        <v>8</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="13">
+        <v>4</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0</v>
+      </c>
+      <c r="N13" s="9">
+        <v>0</v>
+      </c>
+      <c r="O13" s="10">
+        <v>1</v>
+      </c>
+      <c r="P13" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>1</v>
+      </c>
+      <c r="R13" s="10">
+        <v>1</v>
+      </c>
+      <c r="S13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C14" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="8">
+        <f>SUM(E6:E13)</f>
+        <v>80</v>
+      </c>
+      <c r="F14" s="8">
+        <f>E14-($E$14/14)</f>
+        <v>74.285714285714292</v>
+      </c>
+      <c r="G14" s="8">
+        <f>F14-($E$14/14)</f>
+        <v>68.571428571428584</v>
+      </c>
+      <c r="H14" s="8">
+        <f>G14-($E$14/14)</f>
+        <v>62.857142857142868</v>
+      </c>
+      <c r="I14" s="8">
+        <f>H14-($E$14/14)</f>
+        <v>57.142857142857153</v>
+      </c>
+      <c r="J14" s="8">
+        <f>I14-($E$14/14)</f>
+        <v>51.428571428571438</v>
+      </c>
+      <c r="K14" s="8">
+        <f>J14-($E$14/14)</f>
+        <v>45.714285714285722</v>
+      </c>
+      <c r="L14" s="8">
+        <f>K14-($E$14/14)</f>
+        <v>40.000000000000007</v>
+      </c>
+      <c r="M14" s="8">
+        <f>L14-($E$14/14)</f>
+        <v>34.285714285714292</v>
+      </c>
+      <c r="N14" s="8">
+        <f>M14-($E$14/14)</f>
+        <v>28.571428571428577</v>
+      </c>
+      <c r="O14" s="8">
+        <f>N14-($E$14/14)</f>
+        <v>22.857142857142861</v>
+      </c>
+      <c r="P14" s="8">
+        <f>O14-($E$14/14)</f>
+        <v>17.142857142857146</v>
+      </c>
+      <c r="Q14" s="8">
+        <f>P14-($E$14/14)</f>
+        <v>11.428571428571431</v>
+      </c>
+      <c r="R14" s="8">
+        <f>Q14-($E$14/14)</f>
+        <v>5.7142857142857162</v>
+      </c>
+      <c r="S14" s="8">
+        <f>R14-($E$14/14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="8">
+        <f>SUM(E6:E13)</f>
+        <v>80</v>
+      </c>
+      <c r="F15" s="8">
+        <f>E15-SUM(F6:F11)</f>
+        <v>78</v>
+      </c>
+      <c r="G15" s="8">
+        <f>F15-SUM(G6:G11)</f>
+        <v>76</v>
+      </c>
+      <c r="H15" s="8">
+        <f>G15-SUM(H6:H11)</f>
+        <v>74</v>
+      </c>
+      <c r="I15" s="8">
+        <f>H15-SUM(I6:I11)</f>
+        <v>60</v>
+      </c>
+      <c r="J15" s="8">
+        <f>I15-SUM(J6:J11)</f>
+        <v>54</v>
+      </c>
+      <c r="K15" s="8">
+        <f>J15-SUM(K6:K11)</f>
+        <v>50</v>
+      </c>
+      <c r="L15" s="8">
+        <f>K15-SUM(L6:L11)</f>
+        <v>46</v>
+      </c>
+      <c r="M15" s="8">
+        <f>L15-SUM(M6:M11)</f>
+        <v>42</v>
+      </c>
+      <c r="N15" s="8">
+        <f>M15-SUM(N6:N11)</f>
+        <v>34</v>
+      </c>
+      <c r="O15" s="8">
+        <f>N15-SUM(O6:O11)</f>
+        <v>26</v>
+      </c>
+      <c r="P15" s="8">
+        <f>O15-SUM(P6:P11)</f>
+        <v>18</v>
+      </c>
+      <c r="Q15" s="8">
+        <f>P15-SUM(Q6:Q11)</f>
+        <v>11</v>
+      </c>
+      <c r="R15" s="8">
+        <f>Q15-SUM(R6:R11)</f>
+        <v>4</v>
+      </c>
+      <c r="S15" s="8">
+        <f>R15-SUM(S6:S11)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>